<commit_message>
added terminal 100000 to list with globaltel sim
</commit_message>
<xml_diff>
--- a/terminali_dopune_globaltel.xlsx
+++ b/terminali_dopune_globaltel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="307">
   <si>
     <t>R.B.</t>
   </si>
@@ -789,6 +789,162 @@
   </si>
   <si>
     <t>4081</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>8938111000002503604</t>
   </si>
 </sst>
 </file>
@@ -796,7 +952,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="00000"/>
+    <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -879,14 +1035,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1235,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1253,7 +1409,7 @@
     <col min="8" max="1025" width="8.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1276,1153 +1432,1179 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
-        <v>1</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>255</v>
       </c>
       <c r="B2" s="6">
+        <v>354688089433324</v>
+      </c>
+      <c r="C2" s="6">
+        <v>117212608635</v>
+      </c>
+      <c r="D2" s="6">
+        <v>8.9381110000024996E+18</v>
+      </c>
+      <c r="E2" s="6">
+        <v>220117701200359</v>
+      </c>
+      <c r="F2">
+        <v>100000</v>
+      </c>
+      <c r="G2">
+        <v>8657</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" s="6">
         <v>351622076439252</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C3" s="6">
         <v>125191032039</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F3" s="7">
         <v>100101</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F4" s="7">
         <v>100102</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F5" s="7">
         <v>100103</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F6" s="7">
         <v>100104</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F7" s="7">
         <v>100105</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G7" s="9" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F8" s="7">
         <v>100106</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G8" s="9" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
+      <c r="K8" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F9" s="7">
         <v>100107</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G9" s="9" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F10" s="7">
         <v>100108</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F11" s="7">
         <v>100109</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F12" s="7">
         <v>100110</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F13" s="7">
         <v>100111</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F14" s="7">
         <v>100112</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G14" s="9" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F15" s="7">
         <v>100113</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G15" s="9" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F16" s="7">
         <v>100114</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G16" s="9" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F17" s="7">
         <v>100115</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G17" s="9" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <v>16</v>
-      </c>
-      <c r="B17" s="6" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F18" s="7">
         <v>100116</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G18" s="9" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
-        <v>17</v>
-      </c>
-      <c r="B18" s="6" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E19" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F19" s="7">
         <v>100117</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G19" s="9" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <v>18</v>
-      </c>
-      <c r="B19" s="6" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C20" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E20" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F20" s="7">
         <v>100118</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G20" s="9" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C21" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F21" s="7">
         <v>100119</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G21" s="9" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C22" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F22" s="7">
         <v>100120</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G22" s="9" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
-        <v>21</v>
-      </c>
-      <c r="B22" s="6" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F23" s="7">
         <v>100121</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G23" s="9" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
-        <v>22</v>
-      </c>
-      <c r="B23" s="6" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F24" s="7">
         <v>100122</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>23</v>
-      </c>
-      <c r="B24" s="6" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F25" s="7">
         <v>100123</v>
       </c>
-      <c r="G24" s="9" t="s">
+      <c r="G25" s="9" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <v>24</v>
-      </c>
-      <c r="B25" s="6" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E26" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F26" s="7">
         <v>100124</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G26" s="9" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
-        <v>25</v>
-      </c>
-      <c r="B26" s="6" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F27" s="7">
         <v>100125</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="G27" s="9" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
-        <v>26</v>
-      </c>
-      <c r="B27" s="6" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F28" s="7">
         <v>100126</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G28" s="9" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
-        <v>27</v>
-      </c>
-      <c r="B28" s="6" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E29" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F29" s="7">
         <v>100127</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G29" s="9" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
-        <v>28</v>
-      </c>
-      <c r="B29" s="6" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E30" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F30" s="7">
         <v>100128</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G30" s="9" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
-        <v>29</v>
-      </c>
-      <c r="B30" s="6" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E31" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F31" s="7">
         <v>100129</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="G31" s="9" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
-        <v>30</v>
-      </c>
-      <c r="B31" s="6" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E32" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F32" s="7">
         <v>100130</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G32" s="9" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
-        <v>31</v>
-      </c>
-      <c r="B32" s="6" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E33" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F33" s="7">
         <v>100131</v>
       </c>
-      <c r="G32" s="9" t="s">
+      <c r="G33" s="9" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="5">
-        <v>32</v>
-      </c>
-      <c r="B33" s="6" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E34" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F34" s="7">
         <v>100132</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G34" s="9" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
-        <v>33</v>
-      </c>
-      <c r="B34" s="6" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E35" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F35" s="7">
         <v>100133</v>
       </c>
-      <c r="G34" s="9" t="s">
+      <c r="G35" s="9" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
-        <v>34</v>
-      </c>
-      <c r="B35" s="6" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F36" s="7">
         <v>100134</v>
       </c>
-      <c r="G35" s="9" t="s">
+      <c r="G36" s="9" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="5">
-        <v>35</v>
-      </c>
-      <c r="B36" s="6" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D37" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E37" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F37" s="7">
         <v>100135</v>
       </c>
-      <c r="G36" s="9" t="s">
+      <c r="G37" s="9" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="5">
-        <v>36</v>
-      </c>
-      <c r="B37" s="6" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E38" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F38" s="7">
         <v>100136</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G38" s="9" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="5">
-        <v>37</v>
-      </c>
-      <c r="B38" s="6" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D39" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E39" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F39" s="7">
         <v>100137</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G39" s="9" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="5">
-        <v>38</v>
-      </c>
-      <c r="B39" s="6" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E40" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F40" s="7">
         <v>100138</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="G40" s="9" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="5">
-        <v>39</v>
-      </c>
-      <c r="B40" s="6" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C41" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D41" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E41" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F41" s="7">
         <v>100139</v>
       </c>
-      <c r="G40" s="9" t="s">
+      <c r="G41" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="5">
-        <v>40</v>
-      </c>
-      <c r="B41" s="6" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F42" s="7">
         <v>100140</v>
       </c>
-      <c r="G41" s="9" t="s">
+      <c r="G42" s="9" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="5">
-        <v>41</v>
-      </c>
-      <c r="B42" s="6" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B43" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D43" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E43" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F43" s="7">
         <v>100141</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="G43" s="9" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="5">
-        <v>42</v>
-      </c>
-      <c r="B43" s="6" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C44" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D44" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E44" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F44" s="7">
         <v>100142</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="G44" s="9" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="5">
-        <v>43</v>
-      </c>
-      <c r="B44" s="6" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B45" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D45" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E45" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="F44" s="7">
+      <c r="F45" s="7">
         <v>100143</v>
       </c>
-      <c r="G44" s="9" t="s">
+      <c r="G45" s="9" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="5">
-        <v>44</v>
-      </c>
-      <c r="B45" s="6" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D46" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E46" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="F45" s="7">
+      <c r="F46" s="7">
         <v>100144</v>
       </c>
-      <c r="G45" s="9" t="s">
+      <c r="G46" s="9" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="5">
-        <v>45</v>
-      </c>
-      <c r="B46" s="6" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D47" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E47" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F47" s="7">
         <v>100145</v>
       </c>
-      <c r="G46" s="9" t="s">
+      <c r="G47" s="9" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="5">
-        <v>46</v>
-      </c>
-      <c r="B47" s="6" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B48" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C48" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D48" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="E48" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F48" s="7">
         <v>100146</v>
       </c>
-      <c r="G47" s="9" t="s">
+      <c r="G48" s="9" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="5">
-        <v>47</v>
-      </c>
-      <c r="B48" s="6" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C49" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="E48" s="6" t="s">
+      <c r="E49" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="F48" s="7">
+      <c r="F49" s="7">
         <v>100147</v>
       </c>
-      <c r="G48" s="9" t="s">
+      <c r="G49" s="9" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="5">
-        <v>48</v>
-      </c>
-      <c r="B49" s="6" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C50" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D50" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="E50" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="F49" s="7">
+      <c r="F50" s="7">
         <v>100148</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="G50" s="9" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="5">
-        <v>49</v>
-      </c>
-      <c r="B50" s="6" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C51" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="D51" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="E51" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="F50" s="7">
+      <c r="F51" s="7">
         <v>100149</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="G51" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="5">
-        <v>50</v>
-      </c>
-      <c r="B51" s="6" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C52" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D52" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="E52" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="F51" s="7">
+      <c r="F52" s="7">
         <v>100150</v>
       </c>
-      <c r="G51" s="9" t="s">
+      <c r="G52" s="9" t="s">
         <v>254</v>
       </c>
     </row>

</xml_diff>